<commit_message>
Database Excel sheet added
</commit_message>
<xml_diff>
--- a/Database/Notes - MarketPlace Database.xlsx
+++ b/Database/Notes - MarketPlace Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\MarketPlace_Assignments\Notes_MarketPlace_HTML\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="234">
   <si>
     <t>Field Name</t>
   </si>
@@ -2203,6 +2203,41 @@
   </si>
   <si>
     <t xml:space="preserve">status will be updated based on user activity with notes                                                                                                                   Approve - when admin approve the note                                                                                                                                       Reject - when admin Reject the note.                                                                                                                                                  InReview - when admin make note as in-review.  </t>
+  </si>
+  <si>
+    <t>DownloadID</t>
+  </si>
+  <si>
+    <t>BuyerName</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY relationship with Users table. Who buyes this note.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FOREIGN KEY relationship with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> table. Who sells this note.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2460,6 +2495,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2477,12 +2518,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2764,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:E310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="E303" sqref="E303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2783,13 +2818,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
@@ -2804,10 +2839,10 @@
       <c r="A5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
@@ -2960,13 +2995,13 @@
       <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
@@ -5802,13 +5837,13 @@
       <c r="E236" s="3"/>
     </row>
     <row r="239" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A239" s="35" t="s">
+      <c r="A239" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="B239" s="36"/>
-      <c r="C239" s="36"/>
-      <c r="D239" s="36"/>
-      <c r="E239" s="37"/>
+      <c r="B239" s="38"/>
+      <c r="C239" s="38"/>
+      <c r="D239" s="38"/>
+      <c r="E239" s="39"/>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="34" t="s">
@@ -6188,22 +6223,22 @@
       <c r="E268" s="3"/>
     </row>
     <row r="271" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A271" s="35" t="s">
+      <c r="A271" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="B271" s="36"/>
-      <c r="C271" s="36"/>
-      <c r="D271" s="36"/>
-      <c r="E271" s="37"/>
+      <c r="B271" s="38"/>
+      <c r="C271" s="38"/>
+      <c r="D271" s="38"/>
+      <c r="E271" s="39"/>
     </row>
     <row r="272" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="38" t="s">
+      <c r="A272" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="B272" s="39"/>
-      <c r="C272" s="39"/>
-      <c r="D272" s="39"/>
-      <c r="E272" s="40"/>
+      <c r="B272" s="41"/>
+      <c r="C272" s="41"/>
+      <c r="D272" s="41"/>
+      <c r="E272" s="42"/>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="30" t="s">
@@ -6559,7 +6594,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" s="31" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="B301" s="31" t="s">
         <v>5</v>
@@ -6599,112 +6634,145 @@
         <v>15</v>
       </c>
       <c r="E303" s="31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A304" s="31" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B304" s="31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C304" s="2"/>
       <c r="D304" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E304" s="31" t="s">
-        <v>162</v>
+        <v>232</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" s="31" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="B305" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C305" s="31"/>
+      <c r="C305" s="2"/>
       <c r="D305" s="31" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E305" s="31" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A306" s="31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B306" s="31" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C306" s="31"/>
       <c r="D306" s="31" t="s">
         <v>7</v>
       </c>
       <c r="E306" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B307" s="31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C307" s="31"/>
       <c r="D307" s="31" t="s">
         <v>7</v>
       </c>
       <c r="E307" s="31" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B308" s="31" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C308" s="31"/>
       <c r="D308" s="31" t="s">
         <v>7</v>
       </c>
       <c r="E308" s="31" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309" s="31" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B309" s="31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C309" s="31"/>
       <c r="D309" s="31" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E309" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A310" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B310" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C310" s="31"/>
+      <c r="D310" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E310" s="31" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A285:E285"/>
+    <mergeCell ref="A286:E286"/>
+    <mergeCell ref="A271:E271"/>
+    <mergeCell ref="A272:E272"/>
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A240:E240"/>
+    <mergeCell ref="A239:E239"/>
+    <mergeCell ref="A255:E255"/>
+    <mergeCell ref="A256:E256"/>
+    <mergeCell ref="A166:E166"/>
+    <mergeCell ref="A208:E208"/>
+    <mergeCell ref="A209:E209"/>
+    <mergeCell ref="A224:E224"/>
+    <mergeCell ref="A167:E167"/>
+    <mergeCell ref="A180:E180"/>
+    <mergeCell ref="A181:E181"/>
+    <mergeCell ref="A194:E194"/>
+    <mergeCell ref="A195:E195"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A298:E298"/>
     <mergeCell ref="A299:E299"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A64:E64"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A103:E103"/>
     <mergeCell ref="A116:E116"/>
     <mergeCell ref="A115:E115"/>
@@ -6715,24 +6783,6 @@
     <mergeCell ref="A148:E148"/>
     <mergeCell ref="A149:E149"/>
     <mergeCell ref="A129:E129"/>
-    <mergeCell ref="A166:E166"/>
-    <mergeCell ref="A208:E208"/>
-    <mergeCell ref="A209:E209"/>
-    <mergeCell ref="A224:E224"/>
-    <mergeCell ref="A167:E167"/>
-    <mergeCell ref="A180:E180"/>
-    <mergeCell ref="A181:E181"/>
-    <mergeCell ref="A194:E194"/>
-    <mergeCell ref="A195:E195"/>
-    <mergeCell ref="A285:E285"/>
-    <mergeCell ref="A286:E286"/>
-    <mergeCell ref="A271:E271"/>
-    <mergeCell ref="A272:E272"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A240:E240"/>
-    <mergeCell ref="A239:E239"/>
-    <mergeCell ref="A255:E255"/>
-    <mergeCell ref="A256:E256"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>